<commit_message>
master user crud in-progress and two tables removed
</commit_message>
<xml_diff>
--- a/Tours & Travel Management System.xlsx
+++ b/Tours & Travel Management System.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Projects\tours_&amp;_Travels_Management_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AA37AA-774B-4DD9-BF2D-FF40E57DC4F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4A6E0E-A70A-478F-BFB9-97E3CC22D9DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3165" windowHeight="6375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3165" windowHeight="6375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="140">
   <si>
     <t>Travel &amp; tour Management System</t>
   </si>
@@ -206,9 +206,6 @@
     <t>Last Name</t>
   </si>
   <si>
-    <t>state</t>
-  </si>
-  <si>
     <t>city Id</t>
   </si>
   <si>
@@ -349,19 +346,7 @@
     <t>routeIsDeleted</t>
   </si>
   <si>
-    <t>destination stateId</t>
-  </si>
-  <si>
-    <t>source stateId</t>
-  </si>
-  <si>
-    <t>from stateId</t>
-  </si>
-  <si>
     <t>from cityId</t>
-  </si>
-  <si>
-    <t>to stateId</t>
   </si>
   <si>
     <t>to cityId</t>
@@ -456,6 +441,9 @@
   <si>
     <t xml:space="preserve">check how to get backup  and script of tables of mysql database </t>
   </si>
+  <si>
+    <t>master state</t>
+  </si>
 </sst>
 </file>
 
@@ -465,7 +453,7 @@
     <numFmt numFmtId="164" formatCode="d\ mmmm\ yyyy"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -537,12 +525,19 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color theme="6" tint="0.59999389629810485"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="6" tint="0.59999389629810485"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -663,8 +658,14 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1027,11 +1028,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1092,7 +1115,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1120,6 +1142,19 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1154,35 +1189,43 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1405,17 +1448,18 @@
   </sheetPr>
   <dimension ref="A1:AF1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="40.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="46"/>
+    <col min="5" max="5" width="9.5703125" style="45" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" customWidth="1"/>
@@ -1424,19 +1468,19 @@
     <row r="1" spans="1:32" ht="18.75">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="60"/>
+      <c r="D1" s="68"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="70" t="s">
+      <c r="H1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="71"/>
-      <c r="J1" s="72">
+      <c r="I1" s="79"/>
+      <c r="J1" s="80">
         <v>44882</v>
       </c>
-      <c r="K1" s="73"/>
+      <c r="K1" s="81"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -1494,44 +1538,44 @@
       <c r="AF2" s="1"/>
     </row>
     <row r="3" spans="1:32" ht="16.5" thickBot="1">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="61" t="s">
-        <v>141</v>
+      <c r="E3" s="69" t="s">
+        <v>136</v>
       </c>
-      <c r="F3" s="61" t="s">
-        <v>98</v>
+      <c r="F3" s="69" t="s">
+        <v>97</v>
       </c>
-      <c r="G3" s="69" t="s">
+      <c r="G3" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="61" t="s">
+      <c r="H3" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="61" t="s">
+      <c r="I3" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="61" t="s">
+      <c r="J3" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="67" t="s">
+      <c r="K3" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="63" t="s">
+      <c r="L3" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="64"/>
-      <c r="N3" s="65"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="73"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -1552,25 +1596,25 @@
       <c r="AF3" s="1"/>
     </row>
     <row r="4" spans="1:32" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A4" s="66"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="56" t="s">
+      <c r="A4" s="74"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="57" t="s">
+      <c r="M4" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="58" t="s">
-        <v>98</v>
+      <c r="N4" s="57" t="s">
+        <v>97</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -1604,9 +1648,9 @@
       <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52" t="s">
-        <v>99</v>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51" t="s">
+        <v>98</v>
       </c>
       <c r="G5" s="8">
         <v>44861</v>
@@ -1619,14 +1663,14 @@
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
-      <c r="L5" s="49" t="s">
+      <c r="L5" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="54" t="s">
+      <c r="M5" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="55" t="s">
-        <v>99</v>
+      <c r="N5" s="54" t="s">
+        <v>98</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1660,8 +1704,8 @@
       <c r="D6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
       <c r="G6" s="8">
         <v>44861</v>
       </c>
@@ -1672,11 +1716,11 @@
       <c r="L6" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="51" t="s">
+      <c r="M6" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="50" t="s">
-        <v>100</v>
+      <c r="N6" s="49" t="s">
+        <v>99</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -1710,8 +1754,8 @@
       <c r="D7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
       <c r="G7" s="8">
         <v>44861</v>
       </c>
@@ -1758,9 +1802,9 @@
       <c r="D8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52" t="s">
-        <v>99</v>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51" t="s">
+        <v>98</v>
       </c>
       <c r="G8" s="8">
         <v>44861</v>
@@ -1811,11 +1855,11 @@
       <c r="D9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="92">
+      <c r="E9" s="66">
         <v>1</v>
       </c>
-      <c r="F9" s="52" t="s">
-        <v>99</v>
+      <c r="F9" s="51" t="s">
+        <v>98</v>
       </c>
       <c r="G9" s="8">
         <v>44861</v>
@@ -1861,8 +1905,8 @@
       <c r="D10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
       <c r="G10" s="8">
         <v>44861</v>
       </c>
@@ -1905,11 +1949,11 @@
       <c r="D11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="53">
+      <c r="E11" s="52">
         <v>1</v>
       </c>
-      <c r="F11" s="53" t="s">
-        <v>100</v>
+      <c r="F11" s="52" t="s">
+        <v>99</v>
       </c>
       <c r="G11" s="8">
         <v>44861</v>
@@ -1955,8 +1999,8 @@
       <c r="D12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
       <c r="G12" s="8">
         <v>44861</v>
       </c>
@@ -1999,8 +2043,8 @@
       <c r="D13" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
       <c r="G13" s="8">
         <v>44861</v>
       </c>
@@ -2043,8 +2087,8 @@
       <c r="D14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
       <c r="G14" s="8">
         <v>44861</v>
       </c>
@@ -2087,8 +2131,8 @@
       <c r="D15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
       <c r="G15" s="8">
         <v>44861</v>
       </c>
@@ -2131,8 +2175,8 @@
       <c r="D16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
       <c r="G16" s="8">
         <v>44861</v>
       </c>
@@ -2175,8 +2219,8 @@
       <c r="D17" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
       <c r="G17" s="8">
         <v>44861</v>
       </c>
@@ -2219,8 +2263,8 @@
       <c r="D18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
       <c r="G18" s="8">
         <v>44861</v>
       </c>
@@ -2263,9 +2307,9 @@
       <c r="D19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52" t="s">
-        <v>99</v>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51" t="s">
+        <v>98</v>
       </c>
       <c r="G19" s="8">
         <v>44861</v>
@@ -2313,8 +2357,8 @@
       <c r="D20" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
       <c r="G20" s="8">
         <v>44861</v>
       </c>
@@ -2345,25 +2389,25 @@
       <c r="AF20" s="1"/>
     </row>
     <row r="21" spans="1:32" ht="12.75">
-      <c r="A21" s="12">
+      <c r="A21" s="82">
         <v>17</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="11" t="s">
+      <c r="C21" s="84"/>
+      <c r="D21" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="8">
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="87">
         <v>44861</v>
       </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="23"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="84"/>
+      <c r="J21" s="88"/>
+      <c r="K21" s="84"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -2386,36 +2430,36 @@
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
     </row>
-    <row r="22" spans="1:32" s="46" customFormat="1" ht="38.25">
-      <c r="A22" s="87">
+    <row r="22" spans="1:32" s="45" customFormat="1" ht="38.25">
+      <c r="A22" s="89">
         <v>18</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="88" t="s">
-        <v>142</v>
+      <c r="C22" s="94" t="s">
+        <v>137</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="89">
+      <c r="E22" s="92">
         <v>2</v>
       </c>
-      <c r="F22" s="89" t="s">
-        <v>140</v>
+      <c r="F22" s="92" t="s">
+        <v>135</v>
       </c>
-      <c r="G22" s="90">
+      <c r="G22" s="93">
         <v>44865</v>
       </c>
-      <c r="H22" s="90">
+      <c r="H22" s="93">
         <v>44865</v>
       </c>
-      <c r="I22" s="88"/>
-      <c r="J22" s="91" t="s">
-        <v>143</v>
+      <c r="I22" s="49"/>
+      <c r="J22" s="94" t="s">
+        <v>138</v>
       </c>
-      <c r="K22" s="88"/>
+      <c r="K22" s="49"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -35782,6 +35826,7 @@
     <mergeCell ref="E3:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -35792,8 +35837,8 @@
   </sheetPr>
   <dimension ref="B1:N31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -35829,17 +35874,17 @@
       </c>
       <c r="I2" s="28"/>
       <c r="J2" s="29" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
-      <c r="N2" s="78" t="s">
-        <v>102</v>
+      <c r="N2" s="61" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="13.5" thickTop="1">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>45</v>
       </c>
       <c r="C3" s="31" t="s">
@@ -35864,19 +35909,19 @@
         <v>46</v>
       </c>
       <c r="J3" s="32" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="K3" s="31" t="s">
         <v>46</v>
       </c>
       <c r="L3" s="33" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="M3" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="N3" s="75" t="s">
-        <v>101</v>
+      <c r="N3" s="95" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="12.75">
@@ -35897,16 +35942,16 @@
       </c>
       <c r="I4" s="31"/>
       <c r="J4" s="36" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="M4" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="N4" s="74" t="s">
-        <v>103</v>
+      <c r="N4" s="58" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="12.75">
@@ -35926,167 +35971,157 @@
         <v>59</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L5" s="36" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
-      <c r="N5" s="74" t="s">
-        <v>104</v>
+      <c r="N5" s="58" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="12.75">
       <c r="B6" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="36"/>
+      <c r="F6" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="36" t="s">
-        <v>62</v>
-      </c>
       <c r="H6" s="36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I6" s="31"/>
       <c r="J6" s="36" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="L6" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="58"/>
+    </row>
+    <row r="7" spans="2:14" ht="12.75">
+      <c r="B7" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="N6" s="74" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" ht="12.75">
-      <c r="B7" s="37" t="s">
+      <c r="D7" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="F7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="L7" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="N7" s="58" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="12.75">
+      <c r="B8" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="L7" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="N7" s="74" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" ht="12.75">
-      <c r="B8" s="37" t="s">
+      <c r="D8" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="F8" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="H8" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="L8" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="58"/>
+    </row>
+    <row r="9" spans="2:14" ht="12.75">
+      <c r="B9" s="37" t="s">
         <v>69</v>
-      </c>
-      <c r="L8" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="N8" s="74" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" ht="13.5" thickBot="1">
-      <c r="B9" s="37" t="s">
-        <v>70</v>
       </c>
       <c r="F9" s="38"/>
       <c r="H9" s="36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I9" s="39"/>
-      <c r="L9" s="76"/>
-      <c r="N9" s="74" t="s">
+      <c r="L9" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="N9" s="58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="13.5" thickBot="1">
+      <c r="B10" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" s="59"/>
+      <c r="N10" s="58" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B10" s="37" t="s">
+    <row r="11" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B11" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="N10" s="74" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B11" s="37" t="s">
-        <v>74</v>
-      </c>
       <c r="D11" s="40" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E11" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="81" t="s">
-        <v>126</v>
+      <c r="F11" s="96" t="s">
+        <v>121</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J11" s="41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B12" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="L11" s="25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" ht="13.5" thickTop="1">
-      <c r="B12" s="37" t="s">
-        <v>76</v>
-      </c>
       <c r="D12" s="33" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E12" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="82" t="s">
-        <v>128</v>
+      <c r="F12" s="99" t="s">
+        <v>123</v>
       </c>
-      <c r="H12" s="86" t="s">
-        <v>139</v>
+      <c r="H12" s="65" t="s">
+        <v>134</v>
       </c>
-      <c r="I12" s="77" t="s">
+      <c r="I12" s="60" t="s">
         <v>46</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K12" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="L12" s="42" t="s">
-        <v>134</v>
+      <c r="L12" s="101" t="s">
+        <v>128</v>
       </c>
-      <c r="M12" s="31" t="s">
+      <c r="M12" s="97" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="12.75">
-      <c r="B13" s="48" t="s">
-        <v>78</v>
+    <row r="13" spans="2:14" ht="13.5" thickTop="1">
+      <c r="B13" s="47" t="s">
+        <v>77</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="82" t="s">
+      <c r="F13" s="99" t="s">
         <v>45</v>
       </c>
       <c r="H13" s="33" t="s">
@@ -36096,47 +36131,45 @@
         <v>51</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
-      <c r="L13" s="33" t="s">
+      <c r="L13" s="102" t="s">
         <v>129</v>
       </c>
-      <c r="M13" s="31" t="s">
+      <c r="M13" s="97" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="12.75">
       <c r="D14" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E14" s="31"/>
-      <c r="F14" s="82" t="s">
-        <v>129</v>
+      <c r="F14" s="99" t="s">
+        <v>124</v>
       </c>
-      <c r="H14" s="82" t="s">
-        <v>128</v>
+      <c r="H14" s="62" t="s">
+        <v>124</v>
       </c>
       <c r="I14" s="31" t="s">
         <v>51</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
-      <c r="L14" s="86" t="s">
-        <v>139</v>
+      <c r="L14" s="99" t="s">
+        <v>124</v>
       </c>
-      <c r="M14" s="31" t="s">
+      <c r="M14" s="97" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="12.75">
       <c r="D15" s="36" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E15" s="31"/>
-      <c r="F15" s="79" t="s">
-        <v>110</v>
-      </c>
+      <c r="F15" s="103"/>
       <c r="H15" s="33" t="s">
         <v>48</v>
       </c>
@@ -36144,127 +36177,132 @@
         <v>51</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
-      <c r="L15" s="33" t="s">
-        <v>48</v>
+      <c r="L15" s="98" t="s">
+        <v>134</v>
       </c>
-      <c r="M15" s="31" t="s">
+      <c r="M15" s="97" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="13.5" thickBot="1">
       <c r="D16" s="36" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E16" s="31"/>
-      <c r="F16" s="80" t="s">
-        <v>111</v>
+      <c r="F16" s="100" t="s">
+        <v>107</v>
       </c>
       <c r="H16" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I16" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="L16" s="33" t="s">
-        <v>77</v>
+      <c r="L16" s="99" t="s">
+        <v>48</v>
       </c>
-      <c r="M16" s="31" t="s">
+      <c r="M16" s="97" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="14.25" thickTop="1" thickBot="1">
+    <row r="17" spans="2:13" ht="14.25" thickTop="1" thickBot="1">
       <c r="B17" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="80" t="s">
-        <v>112</v>
+      <c r="E17" s="44"/>
+      <c r="F17" s="100"/>
+      <c r="H17" s="42" t="s">
+        <v>76</v>
       </c>
-      <c r="H17" s="43" t="s">
-        <v>77</v>
+      <c r="L17" s="99" t="s">
+        <v>76</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" ht="13.5" thickTop="1">
-      <c r="B18" s="44" t="s">
+      <c r="M17" s="97"/>
+    </row>
+    <row r="18" spans="2:13" ht="13.5" thickTop="1">
+      <c r="B18" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" t="s">
+        <v>139</v>
+      </c>
+      <c r="E18" s="31"/>
+      <c r="F18" s="100" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" s="36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="12.75">
+      <c r="B19" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="100" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" s="36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="12.75">
+      <c r="B20" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="63"/>
+      <c r="F20" s="100" t="s">
+        <v>131</v>
+      </c>
+      <c r="H20" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="80" t="s">
-        <v>113</v>
+    </row>
+    <row r="21" spans="2:13" ht="12.75">
+      <c r="B21" s="36" t="s">
+        <v>92</v>
       </c>
-      <c r="H18" s="36" t="s">
-        <v>84</v>
+      <c r="D21" s="64"/>
+      <c r="F21" s="104" t="s">
+        <v>132</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" ht="12.75">
-      <c r="B19" s="36" t="s">
+      <c r="H21" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="F19" s="80" t="s">
-        <v>132</v>
+    </row>
+    <row r="22" spans="2:13" ht="12.75">
+      <c r="F22" s="100" t="s">
+        <v>133</v>
       </c>
-      <c r="H19" s="36" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="12.75">
-      <c r="B20" s="36" t="s">
+      <c r="H22" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="84"/>
-      <c r="F20" s="80" t="s">
-        <v>136</v>
-      </c>
-      <c r="H20" s="36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="12.75">
-      <c r="B21" s="36" t="s">
+    </row>
+    <row r="23" spans="2:13" ht="12.75"/>
+    <row r="24" spans="2:13" ht="12.75"/>
+    <row r="27" spans="2:13" ht="12.75">
+      <c r="C27" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="85"/>
-      <c r="F21" s="83" t="s">
-        <v>137</v>
+      <c r="E27" s="31" t="s">
+        <v>130</v>
       </c>
-      <c r="H21" s="36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="12.75">
-      <c r="F22" s="80" t="s">
-        <v>138</v>
-      </c>
-      <c r="H22" s="36" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="12.75"/>
-    <row r="24" spans="2:8" ht="12.75"/>
-    <row r="27" spans="2:8" ht="12.75">
-      <c r="C27" s="31" t="s">
+    </row>
+    <row r="28" spans="2:13" ht="12.75">
+      <c r="B28" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="31" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="12.75">
-      <c r="B28" s="31" t="s">
+      <c r="C28" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="31" t="s">
+    </row>
+    <row r="31" spans="2:13" ht="12.75">
+      <c r="B31" s="31" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" ht="12.75">
-      <c r="B31" s="31" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
master tour complected and tomarrow task is assign
</commit_message>
<xml_diff>
--- a/Tours & Travel Management System.xlsx
+++ b/Tours & Travel Management System.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Projects\tours_&amp;_Travels_Management_System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hrushikesh\tours_&amp;_Travels_Management_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4A6E0E-A70A-478F-BFB9-97E3CC22D9DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3165" windowHeight="6375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3165" windowHeight="6375"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="149">
   <si>
     <t>Travel &amp; tour Management System</t>
   </si>
@@ -120,9 +119,6 @@
   </si>
   <si>
     <t>CRUD for vechile driver mapping.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">API's for vechile travel journey. </t>
   </si>
   <si>
     <t>API's for booking history</t>
@@ -391,9 +387,6 @@
     <t>vehicle booking details</t>
   </si>
   <si>
-    <t>mappingvehicleDriverId</t>
-  </si>
-  <si>
     <t>vehicleBookingId</t>
   </si>
   <si>
@@ -444,11 +437,44 @@
   <si>
     <t>master state</t>
   </si>
+  <si>
+    <t>StateName</t>
+  </si>
+  <si>
+    <t>StateIsDeleted</t>
+  </si>
+  <si>
+    <t>StateCode</t>
+  </si>
+  <si>
+    <t>CRUD  for master state.</t>
+  </si>
+  <si>
+    <t>New tables add after review db</t>
+  </si>
+  <si>
+    <t>remove state id from entitiy</t>
+  </si>
+  <si>
+    <t>add route add in the entity</t>
+  </si>
+  <si>
+    <t>after master chnages review this table and then work on it.</t>
+  </si>
+  <si>
+    <t>CRUD for  mappin route cities</t>
+  </si>
+  <si>
+    <t>CRUD for mast hotel</t>
+  </si>
+  <si>
+    <t>vehicleDriverMappingId</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\ mmmm\ yyyy"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
@@ -537,7 +563,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -664,8 +690,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF93C47D"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1050,11 +1088,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1095,10 +1190,7 @@
     <xf numFmtId="0" fontId="9" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1109,9 +1201,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1148,47 +1237,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="19" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1228,6 +1280,67 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1442,15 +1555,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AF1002"/>
+  <dimension ref="A1:AF1004"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1458,7 +1571,7 @@
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="40.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="45" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="41" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
@@ -1468,19 +1581,19 @@
     <row r="1" spans="1:32" ht="18.75">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="68"/>
+      <c r="D1" s="85"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="78" t="s">
+      <c r="H1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="79"/>
-      <c r="J1" s="80">
+      <c r="I1" s="96"/>
+      <c r="J1" s="97">
         <v>44882</v>
       </c>
-      <c r="K1" s="81"/>
+      <c r="K1" s="98"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -1538,44 +1651,44 @@
       <c r="AF2" s="1"/>
     </row>
     <row r="3" spans="1:32" ht="16.5" thickBot="1">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="69" t="s">
-        <v>136</v>
+      <c r="E3" s="86" t="s">
+        <v>134</v>
       </c>
-      <c r="F3" s="69" t="s">
-        <v>97</v>
+      <c r="F3" s="86" t="s">
+        <v>96</v>
       </c>
-      <c r="G3" s="77" t="s">
+      <c r="G3" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="69" t="s">
+      <c r="H3" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="69" t="s">
+      <c r="I3" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="69" t="s">
+      <c r="J3" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="75" t="s">
+      <c r="K3" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="72"/>
-      <c r="N3" s="73"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="90"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -1596,25 +1709,25 @@
       <c r="AF3" s="1"/>
     </row>
     <row r="4" spans="1:32" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A4" s="74"/>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="55" t="s">
+      <c r="A4" s="91"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="56" t="s">
+      <c r="M4" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="57" t="s">
-        <v>97</v>
+      <c r="N4" s="53" t="s">
+        <v>96</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -1645,12 +1758,12 @@
       <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51" t="s">
-        <v>98</v>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47" t="s">
+        <v>97</v>
       </c>
       <c r="G5" s="8">
         <v>44861</v>
@@ -1663,14 +1776,14 @@
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
-      <c r="L5" s="48" t="s">
+      <c r="L5" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="53" t="s">
+      <c r="M5" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="54" t="s">
-        <v>98</v>
+      <c r="N5" s="50" t="s">
+        <v>97</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1704,8 +1817,8 @@
       <c r="D6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
       <c r="G6" s="8">
         <v>44861</v>
       </c>
@@ -1716,11 +1829,11 @@
       <c r="L6" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="50" t="s">
+      <c r="M6" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="49" t="s">
-        <v>99</v>
+      <c r="N6" s="45" t="s">
+        <v>98</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -1754,8 +1867,8 @@
       <c r="D7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
       <c r="G7" s="8">
         <v>44861</v>
       </c>
@@ -1763,7 +1876,7 @@
       <c r="I7" s="13"/>
       <c r="J7" s="14"/>
       <c r="K7" s="15"/>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="117" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="18" t="s">
@@ -1796,15 +1909,15 @@
       <c r="B8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51" t="s">
-        <v>98</v>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47" t="s">
+        <v>97</v>
       </c>
       <c r="G8" s="8">
         <v>44861</v>
@@ -1849,17 +1962,17 @@
       <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>18</v>
+      <c r="D9" s="117" t="s">
+        <v>15</v>
       </c>
-      <c r="E9" s="66">
+      <c r="E9" s="59">
         <v>1</v>
       </c>
-      <c r="F9" s="51" t="s">
-        <v>98</v>
+      <c r="F9" s="47" t="s">
+        <v>97</v>
       </c>
       <c r="G9" s="8">
         <v>44861</v>
@@ -1867,7 +1980,9 @@
       <c r="H9" s="22">
         <v>44865</v>
       </c>
-      <c r="I9" s="13"/>
+      <c r="I9" s="22">
+        <v>44865</v>
+      </c>
       <c r="J9" s="14"/>
       <c r="K9" s="23"/>
       <c r="L9" s="1"/>
@@ -1899,19 +2014,27 @@
       <c r="B10" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>16</v>
+      <c r="D10" s="117" t="s">
+        <v>15</v>
       </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
+      <c r="E10" s="59">
+        <v>1</v>
+      </c>
+      <c r="F10" s="47" t="s">
+        <v>97</v>
+      </c>
       <c r="G10" s="8">
         <v>44861</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
+      <c r="H10" s="22">
+        <v>44865</v>
+      </c>
+      <c r="I10" s="22">
+        <v>44865</v>
+      </c>
       <c r="J10" s="14"/>
       <c r="K10" s="23"/>
       <c r="L10" s="1"/>
@@ -1949,11 +2072,11 @@
       <c r="D11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="48">
         <v>1</v>
       </c>
-      <c r="F11" s="52" t="s">
-        <v>99</v>
+      <c r="F11" s="48" t="s">
+        <v>98</v>
       </c>
       <c r="G11" s="8">
         <v>44861</v>
@@ -1962,7 +2085,9 @@
         <v>44865</v>
       </c>
       <c r="I11" s="13"/>
-      <c r="J11" s="14"/>
+      <c r="J11" s="14" t="s">
+        <v>143</v>
+      </c>
       <c r="K11" s="23"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1993,19 +2118,27 @@
       <c r="B12" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>16</v>
+      <c r="D12" s="7" t="s">
+        <v>15</v>
       </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
+      <c r="E12" s="59">
+        <v>1</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>97</v>
+      </c>
       <c r="G12" s="8">
         <v>44861</v>
       </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
+      <c r="H12" s="22">
+        <v>44865</v>
+      </c>
+      <c r="I12" s="22">
+        <v>44865</v>
+      </c>
       <c r="J12" s="14"/>
       <c r="K12" s="23"/>
       <c r="L12" s="1"/>
@@ -2043,14 +2176,20 @@
       <c r="D13" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="8">
-        <v>44861</v>
+      <c r="E13" s="48">
+        <v>1</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="22">
+        <v>44865</v>
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
-      <c r="J13" s="14"/>
+      <c r="J13" s="15" t="s">
+        <v>143</v>
+      </c>
       <c r="K13" s="23"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -2087,10 +2226,14 @@
       <c r="D14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="8">
-        <v>44861</v>
+      <c r="E14" s="48">
+        <v>1</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="22">
+        <v>44865</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
@@ -2131,10 +2274,14 @@
       <c r="D15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="8">
-        <v>44861</v>
+      <c r="E15" s="48">
+        <v>1</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" s="22">
+        <v>44865</v>
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
@@ -2172,17 +2319,25 @@
       <c r="C16" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>16</v>
+      <c r="D16" s="16" t="s">
+        <v>18</v>
       </c>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="8">
-        <v>44861</v>
+      <c r="E16" s="48">
+        <v>1</v>
       </c>
-      <c r="H16" s="13"/>
+      <c r="F16" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="22">
+        <v>44865</v>
+      </c>
+      <c r="H16" s="118">
+        <v>44866</v>
+      </c>
       <c r="I16" s="13"/>
-      <c r="J16" s="14"/>
+      <c r="J16" s="14" t="s">
+        <v>144</v>
+      </c>
       <c r="K16" s="23"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -2206,27 +2361,31 @@
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
     </row>
-    <row r="17" spans="1:32" ht="12.75">
-      <c r="A17" s="4">
-        <v>13</v>
-      </c>
+    <row r="17" spans="1:32" s="60" customFormat="1" ht="12.75">
+      <c r="A17" s="4"/>
       <c r="B17" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>33</v>
+        <v>146</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>16</v>
+      <c r="D17" s="16" t="s">
+        <v>18</v>
       </c>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="8">
-        <v>44861</v>
+      <c r="E17" s="48">
+        <v>1</v>
       </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="14"/>
+      <c r="F17" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="22">
+        <v>44865</v>
+      </c>
+      <c r="H17" s="118">
+        <v>44866</v>
+      </c>
+      <c r="I17" s="23"/>
+      <c r="J17" s="15"/>
       <c r="K17" s="23"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -2250,27 +2409,29 @@
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
     </row>
-    <row r="18" spans="1:32" ht="12.75">
-      <c r="A18" s="12">
-        <v>14</v>
-      </c>
+    <row r="18" spans="1:32" s="60" customFormat="1" ht="12.75">
+      <c r="A18" s="4"/>
       <c r="B18" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="8">
-        <v>44861</v>
+      <c r="E18" s="48">
+        <v>1</v>
       </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="14"/>
+      <c r="F18" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="22">
+        <v>44865</v>
+      </c>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="15"/>
       <c r="K18" s="23"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -2294,33 +2455,33 @@
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
     </row>
-    <row r="19" spans="1:32" ht="25.5">
-      <c r="A19" s="12">
-        <v>15</v>
+    <row r="19" spans="1:32" ht="12.75">
+      <c r="A19" s="4">
+        <v>13</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>21</v>
+      <c r="B19" s="17" t="s">
+        <v>19</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>35</v>
+      <c r="C19" s="12" t="s">
+        <v>141</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>15</v>
+      <c r="D19" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51" t="s">
+      <c r="E19" s="48">
+        <v>1</v>
+      </c>
+      <c r="F19" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="G19" s="8">
-        <v>44861</v>
+      <c r="G19" s="22">
+        <v>44865</v>
       </c>
-      <c r="H19" s="8">
-        <v>44864</v>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="14" t="s">
+        <v>142</v>
       </c>
-      <c r="I19" s="8">
-        <v>44864</v>
-      </c>
-      <c r="J19" s="14"/>
       <c r="K19" s="23"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -2345,26 +2506,34 @@
       <c r="AF19" s="1"/>
     </row>
     <row r="20" spans="1:32" ht="25.5">
-      <c r="A20" s="4">
-        <v>16</v>
+      <c r="A20" s="12">
+        <v>14</v>
       </c>
-      <c r="B20" s="18" t="s">
-        <v>21</v>
+      <c r="B20" s="17" t="s">
+        <v>19</v>
       </c>
-      <c r="C20" s="19" t="s">
-        <v>36</v>
+      <c r="C20" s="12" t="s">
+        <v>33</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>16</v>
+      <c r="D20" s="16" t="s">
+        <v>18</v>
       </c>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
+      <c r="E20" s="48">
+        <v>1</v>
+      </c>
+      <c r="F20" s="48" t="s">
+        <v>97</v>
+      </c>
       <c r="G20" s="8">
         <v>44861</v>
       </c>
-      <c r="H20" s="13"/>
+      <c r="H20" s="118">
+        <v>44866</v>
+      </c>
       <c r="I20" s="13"/>
-      <c r="J20" s="14"/>
+      <c r="J20" s="114" t="s">
+        <v>145</v>
+      </c>
       <c r="K20" s="23"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -2388,26 +2557,34 @@
       <c r="AE20" s="1"/>
       <c r="AF20" s="1"/>
     </row>
-    <row r="21" spans="1:32" ht="12.75">
-      <c r="A21" s="82">
-        <v>17</v>
+    <row r="21" spans="1:32" ht="25.5">
+      <c r="A21" s="12">
+        <v>15</v>
       </c>
-      <c r="B21" s="83" t="s">
+      <c r="B21" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="84"/>
-      <c r="D21" s="85" t="s">
-        <v>16</v>
+      <c r="C21" s="116" t="s">
+        <v>34</v>
       </c>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="87">
+      <c r="D21" s="117" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="8">
         <v>44861</v>
       </c>
-      <c r="H21" s="84"/>
-      <c r="I21" s="84"/>
-      <c r="J21" s="88"/>
-      <c r="K21" s="84"/>
+      <c r="H21" s="8">
+        <v>44864</v>
+      </c>
+      <c r="I21" s="8">
+        <v>44864</v>
+      </c>
+      <c r="J21" s="14"/>
+      <c r="K21" s="23"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -2430,36 +2607,28 @@
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
     </row>
-    <row r="22" spans="1:32" s="45" customFormat="1" ht="38.25">
-      <c r="A22" s="89">
-        <v>18</v>
-      </c>
-      <c r="B22" s="90" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="94" t="s">
-        <v>137</v>
-      </c>
-      <c r="D22" s="91" t="s">
+    <row r="22" spans="1:32" ht="25.5">
+      <c r="A22" s="4">
         <v>16</v>
       </c>
-      <c r="E22" s="92">
-        <v>2</v>
+      <c r="B22" s="18" t="s">
+        <v>21</v>
       </c>
-      <c r="F22" s="92" t="s">
-        <v>135</v>
+      <c r="C22" s="19" t="s">
+        <v>35</v>
       </c>
-      <c r="G22" s="93">
-        <v>44865</v>
+      <c r="D22" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="H22" s="93">
-        <v>44865</v>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="8">
+        <v>44861</v>
       </c>
-      <c r="I22" s="49"/>
-      <c r="J22" s="94" t="s">
-        <v>138</v>
-      </c>
-      <c r="K22" s="49"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="23"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -2483,17 +2652,25 @@
       <c r="AF22" s="1"/>
     </row>
     <row r="23" spans="1:32" ht="12.75">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
+      <c r="A23" s="61">
+        <v>17</v>
+      </c>
+      <c r="B23" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="63"/>
+      <c r="D23" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="66">
+        <v>44861</v>
+      </c>
+      <c r="H23" s="63"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="63"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -2516,19 +2693,36 @@
       <c r="AE23" s="1"/>
       <c r="AF23" s="1"/>
     </row>
-    <row r="24" spans="1:32" ht="12.75">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2" t="s">
-        <v>37</v>
+    <row r="24" spans="1:32" s="41" customFormat="1" ht="38.25">
+      <c r="A24" s="68">
+        <v>18</v>
       </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
+      <c r="B24" s="69" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="73" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="71">
+        <v>2</v>
+      </c>
+      <c r="F24" s="71" t="s">
+        <v>133</v>
+      </c>
+      <c r="G24" s="72">
+        <v>44865</v>
+      </c>
+      <c r="H24" s="72">
+        <v>44865</v>
+      </c>
+      <c r="I24" s="45"/>
+      <c r="J24" s="73" t="s">
+        <v>136</v>
+      </c>
+      <c r="K24" s="45"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -2553,9 +2747,8 @@
     </row>
     <row r="25" spans="1:32" ht="12.75">
       <c r="A25" s="1"/>
-      <c r="B25" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -2589,7 +2782,7 @@
     <row r="26" spans="1:32" ht="12.75">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -2624,7 +2817,7 @@
     <row r="27" spans="1:32" ht="12.75">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -2658,8 +2851,8 @@
     </row>
     <row r="28" spans="1:32" ht="12.75">
       <c r="A28" s="1"/>
-      <c r="B28" s="24">
-        <v>3</v>
+      <c r="B28" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -2693,8 +2886,9 @@
     </row>
     <row r="29" spans="1:32" ht="12.75">
       <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="B29" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2727,8 +2921,9 @@
     </row>
     <row r="30" spans="1:32" ht="12.75">
       <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="B30" s="24">
+        <v>3</v>
+      </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -35807,6 +36002,74 @@
       <c r="AE1002" s="1"/>
       <c r="AF1002" s="1"/>
     </row>
+    <row r="1003" spans="1:32" ht="12.75">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="1"/>
+      <c r="D1003" s="1"/>
+      <c r="E1003" s="1"/>
+      <c r="F1003" s="1"/>
+      <c r="G1003" s="1"/>
+      <c r="H1003" s="1"/>
+      <c r="I1003" s="1"/>
+      <c r="J1003" s="1"/>
+      <c r="K1003" s="1"/>
+      <c r="L1003" s="1"/>
+      <c r="M1003" s="1"/>
+      <c r="N1003" s="1"/>
+      <c r="O1003" s="1"/>
+      <c r="P1003" s="1"/>
+      <c r="Q1003" s="1"/>
+      <c r="R1003" s="1"/>
+      <c r="S1003" s="1"/>
+      <c r="T1003" s="1"/>
+      <c r="U1003" s="1"/>
+      <c r="V1003" s="1"/>
+      <c r="W1003" s="1"/>
+      <c r="X1003" s="1"/>
+      <c r="Y1003" s="1"/>
+      <c r="Z1003" s="1"/>
+      <c r="AA1003" s="1"/>
+      <c r="AB1003" s="1"/>
+      <c r="AC1003" s="1"/>
+      <c r="AD1003" s="1"/>
+      <c r="AE1003" s="1"/>
+      <c r="AF1003" s="1"/>
+    </row>
+    <row r="1004" spans="1:32" ht="12.75">
+      <c r="A1004" s="1"/>
+      <c r="B1004" s="1"/>
+      <c r="C1004" s="1"/>
+      <c r="D1004" s="1"/>
+      <c r="E1004" s="1"/>
+      <c r="F1004" s="1"/>
+      <c r="G1004" s="1"/>
+      <c r="H1004" s="1"/>
+      <c r="I1004" s="1"/>
+      <c r="J1004" s="1"/>
+      <c r="K1004" s="1"/>
+      <c r="L1004" s="1"/>
+      <c r="M1004" s="1"/>
+      <c r="N1004" s="1"/>
+      <c r="O1004" s="1"/>
+      <c r="P1004" s="1"/>
+      <c r="Q1004" s="1"/>
+      <c r="R1004" s="1"/>
+      <c r="S1004" s="1"/>
+      <c r="T1004" s="1"/>
+      <c r="U1004" s="1"/>
+      <c r="V1004" s="1"/>
+      <c r="W1004" s="1"/>
+      <c r="X1004" s="1"/>
+      <c r="Y1004" s="1"/>
+      <c r="Z1004" s="1"/>
+      <c r="AA1004" s="1"/>
+      <c r="AB1004" s="1"/>
+      <c r="AC1004" s="1"/>
+      <c r="AD1004" s="1"/>
+      <c r="AE1004" s="1"/>
+      <c r="AF1004" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="C1:D1"/>
@@ -35831,14 +36094,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -35858,451 +36121,468 @@
     <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="1" spans="2:14" ht="15.75" customHeight="1" thickBot="1">
+      <c r="D1" s="110"/>
+    </row>
     <row r="2" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
       <c r="B2" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="111"/>
+      <c r="D2" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="F2" s="109" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="H2" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="I2" s="26"/>
+      <c r="J2" s="108" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" s="108" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" ht="13.5" thickTop="1">
+      <c r="B3" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="29" t="s">
-        <v>109</v>
+      <c r="C3" s="28" t="s">
+        <v>45</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="D3" s="107" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="107" t="s">
         <v>110</v>
       </c>
-      <c r="N2" s="61" t="s">
+      <c r="K3" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="M3" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="12.75">
+      <c r="B4" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="28"/>
+      <c r="J4" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="M4" s="28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="12.75">
+      <c r="B5" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="L5" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="12.75">
+      <c r="B6" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="F6" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="28"/>
+      <c r="J6" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="L6" s="33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="12.75">
+      <c r="B7" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="33"/>
+      <c r="L7" s="33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="12.75">
+      <c r="B8" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="35"/>
+      <c r="H8" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="L8" s="34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="13.5" thickBot="1">
+      <c r="B9" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="36"/>
+      <c r="L9" s="33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B10" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" s="55"/>
+    </row>
+    <row r="11" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B11" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="105" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B12" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="54" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="3" spans="2:14" ht="13.5" thickTop="1">
-      <c r="B3" s="46" t="s">
+      <c r="H12" s="106" t="s">
+        <v>132</v>
+      </c>
+      <c r="I12" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="31" t="s">
-        <v>46</v>
+      <c r="J12" s="27" t="s">
+        <v>75</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="K12" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" s="80" t="s">
+        <v>126</v>
+      </c>
+      <c r="M12" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="75" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="13.5" thickTop="1">
+      <c r="B13" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="L13" s="81" t="s">
+        <v>127</v>
+      </c>
+      <c r="M13" s="76" t="s">
+        <v>50</v>
+      </c>
+      <c r="N13" s="78" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="12.75">
+      <c r="D14" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H14" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="I14" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="L14" s="78" t="s">
+        <v>122</v>
+      </c>
+      <c r="M14" s="76" t="s">
+        <v>50</v>
+      </c>
+      <c r="N14" s="78" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="12.75">
+      <c r="D15" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="28"/>
+      <c r="F15" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="K3" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="N3" s="95" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" ht="12.75">
-      <c r="B4" s="35" t="s">
+      <c r="I15" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="31" t="s">
-        <v>51</v>
+      <c r="J15" s="33" t="s">
+        <v>80</v>
       </c>
-      <c r="D4" s="36" t="s">
-        <v>52</v>
+      <c r="L15" s="77" t="s">
+        <v>132</v>
       </c>
-      <c r="F4" s="36" t="s">
-        <v>53</v>
+      <c r="M15" s="76" t="s">
+        <v>50</v>
       </c>
-      <c r="H4" s="36" t="s">
-        <v>54</v>
+      <c r="N15" s="78" t="s">
+        <v>122</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="36" t="s">
-        <v>113</v>
+    </row>
+    <row r="16" spans="2:14" ht="13.5" thickBot="1">
+      <c r="D16" s="33" t="s">
+        <v>123</v>
       </c>
-      <c r="L4" s="32" t="s">
-        <v>114</v>
+      <c r="E16" s="28"/>
+      <c r="F16" s="54" t="s">
+        <v>105</v>
       </c>
-      <c r="M4" s="31" t="s">
-        <v>51</v>
+      <c r="H16" s="30" t="s">
+        <v>79</v>
       </c>
-      <c r="N4" s="58" t="s">
-        <v>102</v>
+      <c r="I16" s="28" t="s">
+        <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="2:14" ht="12.75">
-      <c r="B5" s="37" t="s">
+      <c r="L16" s="78" t="s">
+        <v>47</v>
+      </c>
+      <c r="M16" s="76" t="s">
+        <v>50</v>
+      </c>
+      <c r="N16" s="82"/>
+    </row>
+    <row r="17" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B17" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="40"/>
+      <c r="H17" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="L17" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="M17" s="76"/>
+      <c r="N17" s="79" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B18" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="113"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="28"/>
+      <c r="H18" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="N18" s="79"/>
+    </row>
+    <row r="19" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B19" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="104"/>
+      <c r="D19" s="103" t="s">
+        <v>137</v>
+      </c>
+      <c r="H19" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="N19" s="79" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" ht="13.5" thickTop="1">
+      <c r="B20" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="36" t="s">
-        <v>56</v>
+      <c r="H20" s="33" t="s">
+        <v>86</v>
       </c>
-      <c r="F5" s="36" t="s">
-        <v>57</v>
+      <c r="N20" s="79" t="s">
+        <v>125</v>
       </c>
-      <c r="H5" s="36" t="s">
-        <v>58</v>
+    </row>
+    <row r="21" spans="2:14" ht="12.75">
+      <c r="B21" s="33" t="s">
+        <v>91</v>
       </c>
-      <c r="I5" s="31" t="s">
-        <v>59</v>
+      <c r="D21" s="99" t="s">
+        <v>138</v>
       </c>
-      <c r="J5" s="36" t="s">
-        <v>115</v>
+      <c r="H21" s="33" t="s">
+        <v>88</v>
       </c>
-      <c r="L5" s="36" t="s">
-        <v>116</v>
+      <c r="N21" s="79" t="s">
+        <v>129</v>
       </c>
-      <c r="N5" s="58" t="s">
-        <v>103</v>
+    </row>
+    <row r="22" spans="2:14" ht="12.75">
+      <c r="D22" s="100" t="s">
+        <v>140</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" ht="12.75">
-      <c r="B6" s="37" t="s">
-        <v>60</v>
+      <c r="H22" s="33" t="s">
+        <v>90</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="F6" s="36" t="s">
-        <v>61</v>
+      <c r="N22" s="83" t="s">
+        <v>130</v>
       </c>
-      <c r="H6" s="36" t="s">
-        <v>61</v>
+    </row>
+    <row r="23" spans="2:14" ht="12.75">
+      <c r="D23" s="101" t="s">
+        <v>139</v>
       </c>
-      <c r="I6" s="31"/>
-      <c r="J6" s="36" t="s">
-        <v>117</v>
+      <c r="N23" s="79" t="s">
+        <v>131</v>
       </c>
-      <c r="L6" s="36" t="s">
-        <v>62</v>
+    </row>
+    <row r="24" spans="2:14" ht="12.75"/>
+    <row r="27" spans="2:14" ht="12.75">
+      <c r="C27" s="28" t="s">
+        <v>92</v>
       </c>
-      <c r="N6" s="58"/>
-    </row>
-    <row r="7" spans="2:14" ht="12.75">
-      <c r="B7" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="L7" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="N7" s="58" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" ht="12.75">
-      <c r="B8" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="L8" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="N8" s="58"/>
-    </row>
-    <row r="9" spans="2:14" ht="12.75">
-      <c r="B9" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="38"/>
-      <c r="H9" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="I9" s="39"/>
-      <c r="L9" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="N9" s="58" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="13.5" thickBot="1">
-      <c r="B10" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="L10" s="59"/>
-      <c r="N10" s="58" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B11" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="96" t="s">
-        <v>121</v>
-      </c>
-      <c r="H11" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="J11" s="41" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B12" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="99" t="s">
-        <v>123</v>
-      </c>
-      <c r="H12" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="I12" s="60" t="s">
-        <v>46</v>
-      </c>
-      <c r="J12" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="K12" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="L12" s="101" t="s">
+      <c r="E27" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="M12" s="97" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" ht="13.5" thickTop="1">
-      <c r="B13" s="47" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="99" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="I13" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J13" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="L13" s="102" t="s">
-        <v>129</v>
-      </c>
-      <c r="M13" s="97" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" ht="12.75">
-      <c r="D14" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="99" t="s">
-        <v>124</v>
-      </c>
-      <c r="H14" s="62" t="s">
-        <v>124</v>
-      </c>
-      <c r="I14" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J14" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="L14" s="99" t="s">
-        <v>124</v>
-      </c>
-      <c r="M14" s="97" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" ht="12.75">
-      <c r="D15" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="103"/>
-      <c r="H15" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="I15" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J15" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="L15" s="98" t="s">
-        <v>134</v>
-      </c>
-      <c r="M15" s="97" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" ht="13.5" thickBot="1">
-      <c r="D16" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="100" t="s">
-        <v>107</v>
-      </c>
-      <c r="H16" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="I16" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="L16" s="99" t="s">
-        <v>48</v>
-      </c>
-      <c r="M16" s="97" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B17" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="44"/>
-      <c r="F17" s="100"/>
-      <c r="H17" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="L17" s="99" t="s">
-        <v>76</v>
-      </c>
-      <c r="M17" s="97"/>
-    </row>
-    <row r="18" spans="2:13" ht="13.5" thickTop="1">
-      <c r="B18" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" t="s">
-        <v>139</v>
-      </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="100" t="s">
-        <v>108</v>
-      </c>
-      <c r="H18" s="36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" ht="12.75">
-      <c r="B19" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="100" t="s">
-        <v>127</v>
-      </c>
-      <c r="H19" s="36" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" ht="12.75">
-      <c r="B20" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" s="63"/>
-      <c r="F20" s="100" t="s">
-        <v>131</v>
-      </c>
-      <c r="H20" s="36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" ht="12.75">
-      <c r="B21" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="64"/>
-      <c r="F21" s="104" t="s">
-        <v>132</v>
-      </c>
-      <c r="H21" s="36" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" ht="12.75">
-      <c r="F22" s="100" t="s">
-        <v>133</v>
-      </c>
-      <c r="H22" s="36" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" ht="12.75"/>
-    <row r="24" spans="2:13" ht="12.75"/>
-    <row r="27" spans="2:13" ht="12.75">
-      <c r="C27" s="31" t="s">
+    </row>
+    <row r="28" spans="2:14" ht="12.75">
+      <c r="B28" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" ht="12.75">
-      <c r="B28" s="31" t="s">
+      <c r="C28" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="31" t="s">
+    </row>
+    <row r="31" spans="2:14" ht="12.75">
+      <c r="B31" s="28" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" ht="12.75">
-      <c r="B31" s="31" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CRUD for all masters complected.
</commit_message>
<xml_diff>
--- a/Tours & Travel Management System.xlsx
+++ b/Tours & Travel Management System.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hrushikesh\tours_&amp;_Travels_Management_System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Projects\tours_&amp;_Travels_Management_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA4E135-2A33-4924-8FAA-2930758E1DBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3165" windowHeight="6375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3165" windowHeight="6375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="151">
   <si>
     <t>Travel &amp; tour Management System</t>
   </si>
@@ -230,9 +231,6 @@
   </si>
   <si>
     <t>hotel price</t>
-  </si>
-  <si>
-    <t>booking History</t>
   </si>
   <si>
     <t>address</t>
@@ -462,19 +460,28 @@
     <t>after master chnages review this table and then work on it.</t>
   </si>
   <si>
-    <t>CRUD for  mappin route cities</t>
-  </si>
-  <si>
     <t>CRUD for mast hotel</t>
   </si>
   <si>
     <t>vehicleDriverMappingId</t>
   </si>
+  <si>
+    <t>mappingVechileDriverIsDeleted</t>
+  </si>
+  <si>
+    <t>On-Hold</t>
+  </si>
+  <si>
+    <t>CRUD for  mapping route cities</t>
+  </si>
+  <si>
+    <t>booking History Details</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\ mmmm\ yyyy"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
@@ -563,7 +570,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -592,12 +599,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF9FC5E8"/>
         <bgColor rgb="FF9FC5E8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF93C47D"/>
-        <bgColor rgb="FF93C47D"/>
       </patternFill>
     </fill>
     <fill>
@@ -703,7 +704,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1145,11 +1146,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1158,67 +1179,57 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1235,49 +1246,79 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1313,34 +1354,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1555,15 +1568,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AF1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1571,7 +1584,7 @@
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="40.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="41" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="38" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
@@ -1581,19 +1594,19 @@
     <row r="1" spans="1:32" ht="18.75">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="84" t="s">
+      <c r="C1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="85"/>
+      <c r="D1" s="103"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="95" t="s">
+      <c r="H1" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="96"/>
-      <c r="J1" s="97">
+      <c r="I1" s="114"/>
+      <c r="J1" s="115">
         <v>44882</v>
       </c>
-      <c r="K1" s="98"/>
+      <c r="K1" s="116"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -1651,44 +1664,44 @@
       <c r="AF2" s="1"/>
     </row>
     <row r="3" spans="1:32" ht="16.5" thickBot="1">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="86" t="s">
+      <c r="D3" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="86" t="s">
-        <v>134</v>
+      <c r="E3" s="104" t="s">
+        <v>133</v>
       </c>
-      <c r="F3" s="86" t="s">
-        <v>96</v>
+      <c r="F3" s="104" t="s">
+        <v>95</v>
       </c>
-      <c r="G3" s="94" t="s">
+      <c r="G3" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="86" t="s">
+      <c r="H3" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="86" t="s">
+      <c r="I3" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="86" t="s">
+      <c r="J3" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="92" t="s">
+      <c r="K3" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="88" t="s">
+      <c r="L3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="89"/>
-      <c r="N3" s="90"/>
+      <c r="M3" s="107"/>
+      <c r="N3" s="108"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -1709,25 +1722,25 @@
       <c r="AF3" s="1"/>
     </row>
     <row r="4" spans="1:32" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A4" s="91"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="51" t="s">
+      <c r="A4" s="109"/>
+      <c r="B4" s="109"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="111"/>
+      <c r="L4" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="52" t="s">
+      <c r="M4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="53" t="s">
-        <v>96</v>
+      <c r="N4" s="49" t="s">
+        <v>95</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -1755,35 +1768,35 @@
       <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="117" t="s">
+      <c r="D5" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47" t="s">
-        <v>97</v>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43" t="s">
+        <v>96</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="6">
         <v>44861</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="6">
         <v>44862</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="6">
         <v>44862</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="10"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="8"/>
       <c r="L5" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="49" t="s">
+      <c r="M5" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="50" t="s">
-        <v>97</v>
+      <c r="N5" s="46" t="s">
+        <v>96</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1805,35 +1818,37 @@
       <c r="AF5" s="1"/>
     </row>
     <row r="6" spans="1:32" ht="12.75">
-      <c r="A6" s="12">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="8">
+      <c r="E6" s="44"/>
+      <c r="F6" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="G6" s="6">
         <v>44861</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="16" t="s">
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="46" t="s">
+      <c r="M6" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="45" t="s">
-        <v>98</v>
+      <c r="N6" s="41" t="s">
+        <v>97</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -1855,31 +1870,31 @@
       <c r="AF6" s="1"/>
     </row>
     <row r="7" spans="1:32" ht="12.75">
-      <c r="A7" s="12">
+      <c r="A7" s="9">
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="8">
+      <c r="E7" s="44"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="6">
         <v>44861</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="117" t="s">
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="M7" s="15" t="s">
         <v>21</v>
       </c>
       <c r="N7" s="1"/>
@@ -1906,34 +1921,34 @@
       <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="116" t="s">
+      <c r="C8" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="117" t="s">
+      <c r="D8" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47" t="s">
-        <v>97</v>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43" t="s">
+        <v>96</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="6">
         <v>44861</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="6">
         <v>44862</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="6">
         <v>44862</v>
       </c>
-      <c r="J8" s="14"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="20" t="s">
+      <c r="J8" s="11"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="18" t="s">
         <v>24</v>
       </c>
       <c r="O8" s="1"/>
@@ -1956,35 +1971,35 @@
       <c r="AF8" s="1"/>
     </row>
     <row r="9" spans="1:32" ht="12.75">
-      <c r="A9" s="12">
+      <c r="A9" s="9">
         <v>5</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="115" t="s">
+      <c r="C9" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="117" t="s">
+      <c r="D9" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="59">
+      <c r="E9" s="55">
         <v>1</v>
       </c>
-      <c r="F9" s="47" t="s">
-        <v>97</v>
+      <c r="F9" s="43" t="s">
+        <v>96</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="6">
         <v>44861</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="19">
         <v>44865</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="19">
         <v>44865</v>
       </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="23"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="20"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -2008,35 +2023,35 @@
       <c r="AF9" s="1"/>
     </row>
     <row r="10" spans="1:32" ht="12.75">
-      <c r="A10" s="12">
+      <c r="A10" s="9">
         <v>6</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="115" t="s">
+      <c r="C10" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="117" t="s">
+      <c r="D10" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="59">
+      <c r="E10" s="55">
         <v>1</v>
       </c>
-      <c r="F10" s="47" t="s">
-        <v>97</v>
+      <c r="F10" s="43" t="s">
+        <v>96</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="6">
         <v>44861</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="19">
         <v>44865</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="19">
         <v>44865</v>
       </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="23"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="20"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -2063,32 +2078,32 @@
       <c r="A11" s="4">
         <v>7</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>18</v>
+      <c r="D11" s="96" t="s">
+        <v>15</v>
       </c>
-      <c r="E11" s="48">
+      <c r="E11" s="44">
         <v>1</v>
       </c>
-      <c r="F11" s="48" t="s">
-        <v>98</v>
+      <c r="F11" s="44" t="s">
+        <v>97</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="6">
         <v>44861</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="19">
         <v>44865</v>
       </c>
-      <c r="I11" s="13"/>
-      <c r="J11" s="14" t="s">
-        <v>143</v>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11" t="s">
+        <v>142</v>
       </c>
-      <c r="K11" s="23"/>
+      <c r="K11" s="20"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -2112,35 +2127,35 @@
       <c r="AF11" s="1"/>
     </row>
     <row r="12" spans="1:32" ht="12.75">
-      <c r="A12" s="12">
+      <c r="A12" s="9">
         <v>8</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="115" t="s">
+      <c r="C12" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="59">
+      <c r="E12" s="55">
         <v>1</v>
       </c>
-      <c r="F12" s="47" t="s">
-        <v>97</v>
+      <c r="F12" s="43" t="s">
+        <v>96</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="6">
         <v>44861</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="19">
         <v>44865</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="19">
         <v>44865</v>
       </c>
-      <c r="J12" s="14"/>
-      <c r="K12" s="23"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="20"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -2164,33 +2179,35 @@
       <c r="AF12" s="1"/>
     </row>
     <row r="13" spans="1:32" ht="12.75">
-      <c r="A13" s="12">
+      <c r="A13" s="9">
         <v>9</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>16</v>
+      <c r="D13" s="96" t="s">
+        <v>15</v>
       </c>
-      <c r="E13" s="48">
+      <c r="E13" s="44">
         <v>1</v>
       </c>
-      <c r="F13" s="48" t="s">
-        <v>98</v>
+      <c r="F13" s="44" t="s">
+        <v>97</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="19">
         <v>44865</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="15" t="s">
-        <v>143</v>
+      <c r="H13" s="97">
+        <v>44866</v>
       </c>
-      <c r="K13" s="23"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="K13" s="20"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -2217,28 +2234,30 @@
       <c r="A14" s="4">
         <v>10</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>16</v>
+      <c r="D14" s="13" t="s">
+        <v>18</v>
       </c>
-      <c r="E14" s="48">
+      <c r="E14" s="44">
         <v>1</v>
       </c>
-      <c r="F14" s="48" t="s">
-        <v>98</v>
+      <c r="F14" s="44" t="s">
+        <v>97</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="19">
         <v>44865</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="23"/>
+      <c r="H14" s="97">
+        <v>44866</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="20"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -2262,31 +2281,33 @@
       <c r="AF14" s="1"/>
     </row>
     <row r="15" spans="1:32" ht="12.75">
-      <c r="A15" s="12">
+      <c r="A15" s="9">
         <v>11</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>16</v>
+      <c r="D15" s="96" t="s">
+        <v>15</v>
       </c>
-      <c r="E15" s="48">
+      <c r="E15" s="44">
         <v>1</v>
       </c>
-      <c r="F15" s="48" t="s">
-        <v>98</v>
+      <c r="F15" s="44" t="s">
+        <v>97</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="19">
         <v>44865</v>
       </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="23"/>
+      <c r="H15" s="97">
+        <v>44866</v>
+      </c>
+      <c r="I15" s="10"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="20"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -2310,35 +2331,35 @@
       <c r="AF15" s="1"/>
     </row>
     <row r="16" spans="1:32" ht="12.75">
-      <c r="A16" s="12">
+      <c r="A16" s="9">
         <v>12</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>18</v>
+      <c r="D16" s="96" t="s">
+        <v>15</v>
       </c>
-      <c r="E16" s="48">
+      <c r="E16" s="44">
         <v>1</v>
       </c>
-      <c r="F16" s="48" t="s">
-        <v>97</v>
+      <c r="F16" s="44" t="s">
+        <v>96</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="19">
         <v>44865</v>
       </c>
-      <c r="H16" s="118">
+      <c r="H16" s="97">
         <v>44866</v>
       </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="14" t="s">
-        <v>144</v>
+      <c r="I16" s="10"/>
+      <c r="J16" s="11" t="s">
+        <v>143</v>
       </c>
-      <c r="K16" s="23"/>
+      <c r="K16" s="20"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -2361,32 +2382,32 @@
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
     </row>
-    <row r="17" spans="1:32" s="60" customFormat="1" ht="12.75">
+    <row r="17" spans="1:32" s="56" customFormat="1" ht="12.75">
       <c r="A17" s="4"/>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>146</v>
+      <c r="C17" s="94" t="s">
+        <v>149</v>
       </c>
-      <c r="D17" s="16" t="s">
-        <v>18</v>
+      <c r="D17" s="96" t="s">
+        <v>15</v>
       </c>
-      <c r="E17" s="48">
+      <c r="E17" s="44">
         <v>1</v>
       </c>
-      <c r="F17" s="48" t="s">
-        <v>97</v>
+      <c r="F17" s="44" t="s">
+        <v>96</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="19">
         <v>44865</v>
       </c>
-      <c r="H17" s="118">
+      <c r="H17" s="97">
         <v>44866</v>
       </c>
-      <c r="I17" s="23"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="23"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="20"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -2409,30 +2430,30 @@
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
     </row>
-    <row r="18" spans="1:32" s="60" customFormat="1" ht="12.75">
+    <row r="18" spans="1:32" s="56" customFormat="1" ht="12.75">
       <c r="A18" s="4"/>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>147</v>
+      <c r="C18" s="9" t="s">
+        <v>145</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>16</v>
+      <c r="D18" s="44" t="s">
+        <v>148</v>
       </c>
-      <c r="E18" s="48">
+      <c r="E18" s="44">
         <v>1</v>
       </c>
-      <c r="F18" s="48" t="s">
-        <v>98</v>
+      <c r="F18" s="44" t="s">
+        <v>97</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="19">
         <v>44865</v>
       </c>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="23"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="20"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -2459,30 +2480,32 @@
       <c r="A19" s="4">
         <v>13</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="44">
+        <v>1</v>
+      </c>
+      <c r="F19" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" s="19">
+        <v>44865</v>
+      </c>
+      <c r="H19" s="97">
+        <v>44866</v>
+      </c>
+      <c r="I19" s="10"/>
+      <c r="J19" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="48">
-        <v>1</v>
-      </c>
-      <c r="F19" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" s="22">
-        <v>44865</v>
-      </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="K19" s="23"/>
+      <c r="K19" s="20"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -2506,35 +2529,35 @@
       <c r="AF19" s="1"/>
     </row>
     <row r="20" spans="1:32" ht="25.5">
-      <c r="A20" s="12">
+      <c r="A20" s="9">
         <v>14</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="16" t="s">
-        <v>18</v>
+      <c r="D20" s="96" t="s">
+        <v>15</v>
       </c>
-      <c r="E20" s="48">
+      <c r="E20" s="44">
         <v>1</v>
       </c>
-      <c r="F20" s="48" t="s">
-        <v>97</v>
+      <c r="F20" s="44" t="s">
+        <v>96</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="6">
         <v>44861</v>
       </c>
-      <c r="H20" s="118">
+      <c r="H20" s="97">
         <v>44866</v>
       </c>
-      <c r="I20" s="13"/>
-      <c r="J20" s="114" t="s">
-        <v>145</v>
+      <c r="I20" s="10"/>
+      <c r="J20" s="93" t="s">
+        <v>144</v>
       </c>
-      <c r="K20" s="23"/>
+      <c r="K20" s="20"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -2558,33 +2581,35 @@
       <c r="AF20" s="1"/>
     </row>
     <row r="21" spans="1:32" ht="25.5">
-      <c r="A21" s="12">
+      <c r="A21" s="9">
         <v>15</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="116" t="s">
+      <c r="C21" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="117" t="s">
+      <c r="D21" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47" t="s">
-        <v>97</v>
+      <c r="E21" s="101">
+        <v>1</v>
       </c>
-      <c r="G21" s="8">
+      <c r="F21" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="6">
         <v>44861</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="6">
         <v>44864</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="6">
         <v>44864</v>
       </c>
-      <c r="J21" s="14"/>
-      <c r="K21" s="23"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="20"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -2611,24 +2636,24 @@
       <c r="A22" s="4">
         <v>16</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="8">
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="6">
         <v>44861</v>
       </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="23"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="20"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -2652,25 +2677,25 @@
       <c r="AF22" s="1"/>
     </row>
     <row r="23" spans="1:32" ht="12.75">
-      <c r="A23" s="61">
+      <c r="A23" s="57">
         <v>17</v>
       </c>
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="63"/>
-      <c r="D23" s="64" t="s">
+      <c r="C23" s="59"/>
+      <c r="D23" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66">
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="61">
         <v>44861</v>
       </c>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="63"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="59"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -2693,36 +2718,36 @@
       <c r="AE23" s="1"/>
       <c r="AF23" s="1"/>
     </row>
-    <row r="24" spans="1:32" s="41" customFormat="1" ht="38.25">
-      <c r="A24" s="68">
+    <row r="24" spans="1:32" s="38" customFormat="1" ht="38.25">
+      <c r="A24" s="63">
         <v>18</v>
       </c>
-      <c r="B24" s="69" t="s">
+      <c r="B24" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="73" t="s">
+      <c r="C24" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="65">
+        <v>2</v>
+      </c>
+      <c r="F24" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="66">
+        <v>44865</v>
+      </c>
+      <c r="H24" s="66">
+        <v>44865</v>
+      </c>
+      <c r="I24" s="41"/>
+      <c r="J24" s="67" t="s">
         <v>135</v>
       </c>
-      <c r="D24" s="70" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="71">
-        <v>2</v>
-      </c>
-      <c r="F24" s="71" t="s">
-        <v>133</v>
-      </c>
-      <c r="G24" s="72">
-        <v>44865</v>
-      </c>
-      <c r="H24" s="72">
-        <v>44865</v>
-      </c>
-      <c r="I24" s="45"/>
-      <c r="J24" s="73" t="s">
-        <v>136</v>
-      </c>
-      <c r="K24" s="45"/>
+      <c r="K24" s="41"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -2921,7 +2946,7 @@
     </row>
     <row r="30" spans="1:32" ht="12.75">
       <c r="A30" s="1"/>
-      <c r="B30" s="24">
+      <c r="B30" s="21">
         <v>3</v>
       </c>
       <c r="D30" s="1"/>
@@ -36094,14 +36119,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B1:N31"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -36122,467 +36147,470 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D1" s="110"/>
+      <c r="D1" s="89"/>
     </row>
     <row r="2" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="112" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="109" t="s">
+      <c r="F2" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="109" t="s">
+      <c r="H2" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="108" t="s">
+      <c r="I2" s="23"/>
+      <c r="J2" s="87" t="s">
+        <v>107</v>
+      </c>
+      <c r="L2" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="L2" s="108" t="s">
+    </row>
+    <row r="3" spans="2:14" ht="13.5" thickTop="1">
+      <c r="B3" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="86" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="86" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="3" spans="2:14" ht="13.5" thickTop="1">
-      <c r="B3" s="42" t="s">
+      <c r="K3" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="M3" s="25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="12.75">
+      <c r="B4" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="25"/>
+      <c r="J4" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="L4" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="12.75">
+      <c r="B5" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="12.75">
+      <c r="B6" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="25"/>
+      <c r="J6" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="L6" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="12.75">
+      <c r="B7" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="L7" s="30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="12.75">
+      <c r="B8" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="H8" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="13.5" thickBot="1">
+      <c r="B9" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="33"/>
+      <c r="L9" s="30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B10" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="84" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="84" t="s">
+        <v>150</v>
+      </c>
+      <c r="L10" s="51"/>
+    </row>
+    <row r="11" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B11" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" s="85" t="s">
+        <v>131</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B12" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="H12" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="I12" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="107" t="s">
-        <v>46</v>
+      <c r="J12" s="24" t="s">
+        <v>74</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="K12" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="L12" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="M12" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="69" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="13.5" thickTop="1">
+      <c r="B13" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="L13" s="75" t="s">
+        <v>126</v>
+      </c>
+      <c r="M13" s="70" t="s">
+        <v>50</v>
+      </c>
+      <c r="N13" s="72" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="12.75">
+      <c r="D14" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="25"/>
+      <c r="F14" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="I14" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="L14" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="M14" s="70" t="s">
+        <v>50</v>
+      </c>
+      <c r="N14" s="72" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="12.75">
+      <c r="D15" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="E15" s="25"/>
+      <c r="F15" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="L15" s="71" t="s">
+        <v>131</v>
+      </c>
+      <c r="M15" s="70" t="s">
+        <v>50</v>
+      </c>
+      <c r="N15" s="72" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="13.5" thickBot="1">
+      <c r="D16" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="E16" s="25"/>
+      <c r="F16" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="M16" s="70" t="s">
+        <v>50</v>
+      </c>
+      <c r="N16" s="76"/>
+    </row>
+    <row r="17" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B17" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="27" t="s">
-        <v>48</v>
+      <c r="D17" s="78" t="s">
+        <v>147</v>
       </c>
-      <c r="I3" s="31" t="s">
-        <v>45</v>
+      <c r="E17" s="37"/>
+      <c r="H17" s="30" t="s">
+        <v>81</v>
       </c>
-      <c r="J3" s="107" t="s">
-        <v>110</v>
+      <c r="L17" s="72" t="s">
+        <v>74</v>
       </c>
-      <c r="K3" s="28" t="s">
-        <v>45</v>
+      <c r="M17" s="70"/>
+      <c r="N17" s="73" t="s">
+        <v>105</v>
       </c>
-      <c r="L3" s="27" t="s">
-        <v>111</v>
+    </row>
+    <row r="18" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B18" s="36" t="s">
+        <v>84</v>
       </c>
-      <c r="M3" s="28" t="s">
-        <v>45</v>
+      <c r="C18" s="99"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="100"/>
+      <c r="H18" s="30" t="s">
+        <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="2:14" ht="12.75">
-      <c r="B4" s="32" t="s">
-        <v>49</v>
+      <c r="N18" s="73"/>
+    </row>
+    <row r="19" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B19" s="30" t="s">
+        <v>86</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>50</v>
+      <c r="C19" s="92"/>
+      <c r="D19" s="82" t="s">
+        <v>136</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>51</v>
+      <c r="H19" s="30" t="s">
+        <v>85</v>
       </c>
-      <c r="F4" s="33" t="s">
-        <v>52</v>
+      <c r="N19" s="73" t="s">
+        <v>106</v>
       </c>
-      <c r="H4" s="33" t="s">
-        <v>53</v>
+    </row>
+    <row r="20" spans="2:14" ht="13.5" thickTop="1">
+      <c r="B20" s="30" t="s">
+        <v>88</v>
       </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="L4" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="M4" s="28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" ht="12.75">
-      <c r="B5" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="33" t="s">
+      <c r="C20" s="83"/>
+      <c r="D20" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="33" t="s">
-        <v>56</v>
+      <c r="H20" s="30" t="s">
+        <v>87</v>
       </c>
-      <c r="H5" s="33" t="s">
-        <v>57</v>
+      <c r="N20" s="73" t="s">
+        <v>124</v>
       </c>
-      <c r="I5" s="28" t="s">
-        <v>58</v>
+    </row>
+    <row r="21" spans="2:14" ht="12.75">
+      <c r="B21" s="30" t="s">
+        <v>90</v>
       </c>
-      <c r="J5" s="33" t="s">
-        <v>114</v>
+      <c r="D21" s="78" t="s">
+        <v>137</v>
       </c>
-      <c r="L5" s="33" t="s">
-        <v>115</v>
+      <c r="H21" s="30" t="s">
+        <v>89</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" ht="12.75">
-      <c r="B6" s="34" t="s">
-        <v>59</v>
+      <c r="N21" s="73" t="s">
+        <v>128</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="F6" s="33" t="s">
-        <v>60</v>
+    </row>
+    <row r="22" spans="2:14" ht="12.75">
+      <c r="D22" s="79" t="s">
+        <v>139</v>
       </c>
-      <c r="H6" s="33" t="s">
-        <v>60</v>
+      <c r="N22" s="77" t="s">
+        <v>129</v>
       </c>
-      <c r="I6" s="28"/>
-      <c r="J6" s="33" t="s">
-        <v>116</v>
+    </row>
+    <row r="23" spans="2:14" ht="12.75">
+      <c r="D23" s="80" t="s">
+        <v>138</v>
       </c>
-      <c r="L6" s="33" t="s">
-        <v>61</v>
+      <c r="N23" s="73" t="s">
+        <v>130</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="12.75">
-      <c r="B7" s="34" t="s">
-        <v>62</v>
+    <row r="24" spans="2:14" ht="12.75"/>
+    <row r="27" spans="2:14" ht="12.75">
+      <c r="C27" s="25" t="s">
+        <v>91</v>
       </c>
-      <c r="D7" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" s="33"/>
-      <c r="L7" s="33" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" ht="12.75">
-      <c r="B8" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="35"/>
-      <c r="H8" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="L8" s="34" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" ht="13.5" thickBot="1">
-      <c r="B9" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="I9" s="36"/>
-      <c r="L9" s="33" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B10" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="57" t="s">
-        <v>100</v>
-      </c>
-      <c r="L10" s="55"/>
-    </row>
-    <row r="11" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B11" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="105" t="s">
-        <v>119</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="74" t="s">
-        <v>99</v>
-      </c>
-      <c r="H11" s="105" t="s">
-        <v>70</v>
-      </c>
-      <c r="J11" s="37" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B12" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="54" t="s">
-        <v>101</v>
-      </c>
-      <c r="H12" s="106" t="s">
-        <v>132</v>
-      </c>
-      <c r="I12" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="K12" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="L12" s="80" t="s">
-        <v>126</v>
-      </c>
-      <c r="M12" s="76" t="s">
-        <v>45</v>
-      </c>
-      <c r="N12" s="75" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" ht="13.5" thickTop="1">
-      <c r="B13" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="54" t="s">
-        <v>102</v>
-      </c>
-      <c r="H13" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="I13" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="J13" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="L13" s="81" t="s">
+      <c r="E27" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="M13" s="76" t="s">
-        <v>50</v>
-      </c>
-      <c r="N13" s="78" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" ht="12.75">
-      <c r="D14" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H14" s="58" t="s">
-        <v>122</v>
-      </c>
-      <c r="I14" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="J14" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="L14" s="78" t="s">
-        <v>122</v>
-      </c>
-      <c r="M14" s="76" t="s">
-        <v>50</v>
-      </c>
-      <c r="N14" s="78" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" ht="12.75">
-      <c r="D15" s="74" t="s">
-        <v>99</v>
-      </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="54" t="s">
-        <v>104</v>
-      </c>
-      <c r="H15" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="J15" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="L15" s="77" t="s">
-        <v>132</v>
-      </c>
-      <c r="M15" s="76" t="s">
-        <v>50</v>
-      </c>
-      <c r="N15" s="78" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" ht="13.5" thickBot="1">
-      <c r="D16" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" s="28"/>
-      <c r="F16" s="54" t="s">
-        <v>105</v>
-      </c>
-      <c r="H16" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="I16" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="L16" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="M16" s="76" t="s">
-        <v>50</v>
-      </c>
-      <c r="N16" s="82"/>
-    </row>
-    <row r="17" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B17" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="E17" s="40"/>
-      <c r="H17" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="L17" s="78" t="s">
-        <v>75</v>
-      </c>
-      <c r="M17" s="76"/>
-      <c r="N17" s="79" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B18" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="113"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="28"/>
-      <c r="H18" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="N18" s="79"/>
-    </row>
-    <row r="19" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B19" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="104"/>
-      <c r="D19" s="103" t="s">
-        <v>137</v>
-      </c>
-      <c r="H19" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="N19" s="79" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" ht="13.5" thickTop="1">
-      <c r="B20" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" s="102" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="N20" s="79" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" ht="12.75">
-      <c r="B21" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" s="99" t="s">
-        <v>138</v>
-      </c>
-      <c r="H21" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="N21" s="79" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" ht="12.75">
-      <c r="D22" s="100" t="s">
-        <v>140</v>
-      </c>
-      <c r="H22" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="N22" s="83" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" ht="12.75">
-      <c r="D23" s="101" t="s">
-        <v>139</v>
-      </c>
-      <c r="N23" s="79" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" ht="12.75"/>
-    <row r="27" spans="2:14" ht="12.75">
-      <c r="C27" s="28" t="s">
+    </row>
+    <row r="28" spans="2:14" ht="12.75">
+      <c r="B28" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="E27" s="28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" ht="12.75">
-      <c r="B28" s="28" t="s">
+      <c r="C28" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C28" s="28" t="s">
+    </row>
+    <row r="31" spans="2:14" ht="12.75">
+      <c r="B31" s="25" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" ht="12.75">
-      <c r="B31" s="28" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>